<commit_message>
new logistic regression run
</commit_message>
<xml_diff>
--- a/Output/Classifier Fitting/Logistic Regression/All_Data Training Statistics.xlsx
+++ b/Output/Classifier Fitting/Logistic Regression/All_Data Training Statistics.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.07560424407323202</v>
+        <v>1503.614180982113</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001260070734553867</v>
+        <v>0.2504771249345515</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8166666666666667</v>
+        <v>0.9841745793769782</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7000000000000001</v>
+        <v>0.915708021093533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>